<commit_message>
Technisches Pflichtenheft Einleitung V1
</commit_message>
<xml_diff>
--- a/Hardware/LED_Evaluation.xlsx
+++ b/Hardware/LED_Evaluation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silva\OneDrive\pro4E\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgaer\Google Drive\Fachhochschule\4.Semester\pro4E\gitHub\pro4e\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="6_{A74443D5-16BA-4B7D-BF15-5B4478B8E4B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{94CD4482-C5F2-4BCA-80F0-AFD2AC4162D5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA306DD-6E68-48F2-A2E6-843AC848EBEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DFDA4EE7-2649-4A6F-B313-8DACCA054B93}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{DFDA4EE7-2649-4A6F-B313-8DACCA054B93}"/>
   </bookViews>
   <sheets>
     <sheet name="LED Evaluation" sheetId="1" r:id="rId1"/>
     <sheet name="Stückliste" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -982,25 +982,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C137992A-754F-40DD-9A0A-70F200EDDDD2}">
   <dimension ref="B1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.07421875" customWidth="1"/>
+    <col min="2" max="2" width="35.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.07421875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.88671875" style="30" customWidth="1"/>
+    <col min="5" max="5" width="12.07421875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.84375" style="30" customWidth="1"/>
     <col min="7" max="7" width="9" style="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
-    <col min="9" max="9" width="4.88671875" customWidth="1"/>
+    <col min="9" max="9" width="4.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="20" t="s">
         <v>13</v>
       </c>
@@ -1012,7 +1012,7 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="E3" s="1"/>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
@@ -1035,7 +1035,7 @@
       <c r="E4" s="1"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="E5" s="1"/>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="23" t="s">
         <v>11</v>
       </c>
@@ -1060,8 +1060,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="20" t="s">
         <v>3</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B9" s="21" t="s">
         <v>6</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B10" s="22" t="s">
         <v>7</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B11" s="22" t="s">
         <v>19</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B12" s="22" t="s">
         <v>14</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B13" s="22" t="s">
         <v>32</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B14" s="22" t="s">
         <v>8</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B16" s="22" t="s">
         <v>9</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B17" s="22" t="s">
         <v>10</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>4710</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="23" t="s">
         <v>22</v>
       </c>
@@ -1275,8 +1275,8 @@
         <v>212.31422505307856</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="20" t="s">
         <v>28</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B21" s="21" t="s">
         <v>20</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B22" s="22" t="s">
         <v>26</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B23" s="22" t="s">
         <v>27</v>
       </c>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="H23" s="30"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B24" s="22" t="s">
         <v>21</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>309.40594059405942</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" s="49" t="s">
         <v>23</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>15.222720000000001</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="23" t="s">
         <v>29</v>
       </c>
@@ -1418,8 +1418,8 @@
         <v>30.445440000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B28" s="34" t="s">
         <v>16</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B29" s="32" t="s">
         <v>15</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B30" s="33" t="s">
         <v>17</v>
       </c>
@@ -1483,19 +1483,19 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.4609375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>40</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>37</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>29.0976</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>1.919</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>33</v>
       </c>
@@ -1584,21 +1584,21 @@
         <v>4.4820000000000002</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F8" s="55"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F9" s="55">
         <f>SUM(F4:F8)</f>
         <v>86.09859999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>40</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>29.0976</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>42</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>6.78</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>33</v>
       </c>
@@ -1687,21 +1687,21 @@
         <v>4.4820000000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F17" s="55"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F18" s="55">
         <f>SUM(F13:F17)</f>
         <v>90.959599999999995</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>40</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>43</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>12.25</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
         <v>34</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>1.919</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>33</v>
       </c>
@@ -1790,10 +1790,10 @@
         <v>4.4820000000000002</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F26" s="55"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.4">
       <c r="F27" s="55">
         <f>SUM(F22:F26)</f>
         <v>69.251000000000005</v>

</xml_diff>